<commit_message>
data: add latest data
</commit_message>
<xml_diff>
--- a/out/2023-02-25_cb_list.xlsx
+++ b/out/2023-02-25_cb_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15560"/>
+    <workbookView windowHeight="15560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -10349,12 +10349,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10379,9 +10379,40 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10418,35 +10449,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -10455,7 +10457,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10470,22 +10479,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10500,24 +10501,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -10530,7 +10523,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10542,25 +10643,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10572,25 +10655,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10602,13 +10673,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10620,97 +10697,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10748,17 +10741,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10772,13 +10765,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10798,17 +10795,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10839,155 +10832,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -11337,7 +11336,7 @@
   <sheetPr/>
   <dimension ref="A1:AG488"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -61078,53 +61077,56 @@
   <sheetPr/>
   <dimension ref="A1:AG12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <cols>
+    <col min="15" max="15" width="58.203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:33">
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="32" customHeight="1" spans="2:33">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -61182,7 +61184,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" ht="34" spans="1:33">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -61225,7 +61227,7 @@
       <c r="N2" t="s">
         <v>38</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="3" t="s">
         <v>1552</v>
       </c>
       <c r="P2">
@@ -61283,7 +61285,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" ht="34" spans="1:33">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -61326,7 +61328,7 @@
       <c r="N3" t="s">
         <v>38</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="3" t="s">
         <v>1637</v>
       </c>
       <c r="P3">
@@ -61384,7 +61386,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" ht="34" spans="1:33">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -61427,7 +61429,7 @@
       <c r="N4" t="s">
         <v>38</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="3" t="s">
         <v>1756</v>
       </c>
       <c r="P4">
@@ -61485,7 +61487,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" ht="34" spans="1:33">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -61528,7 +61530,7 @@
       <c r="N5" t="s">
         <v>38</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="3" t="s">
         <v>2227</v>
       </c>
       <c r="P5">
@@ -61586,7 +61588,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" ht="34" spans="1:33">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -61629,7 +61631,7 @@
       <c r="N6" t="s">
         <v>38</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="3" t="s">
         <v>2322</v>
       </c>
       <c r="P6">
@@ -61687,7 +61689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" ht="34" spans="1:33">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -61730,7 +61732,7 @@
       <c r="N7" t="s">
         <v>38</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="3" t="s">
         <v>2551</v>
       </c>
       <c r="P7">
@@ -61788,7 +61790,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" ht="34" spans="1:33">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -61831,7 +61833,7 @@
       <c r="N8" t="s">
         <v>38</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="3" t="s">
         <v>2788</v>
       </c>
       <c r="P8">
@@ -61889,7 +61891,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" ht="51" spans="1:33">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -61932,7 +61934,7 @@
       <c r="N9" t="s">
         <v>38</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="3" t="s">
         <v>2858</v>
       </c>
       <c r="P9">
@@ -61990,7 +61992,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" ht="34" spans="1:33">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -62033,7 +62035,7 @@
       <c r="N10" t="s">
         <v>38</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="3" t="s">
         <v>3019</v>
       </c>
       <c r="P10">
@@ -62091,7 +62093,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" ht="51" spans="1:33">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -62134,7 +62136,7 @@
       <c r="N11" t="s">
         <v>38</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="3" t="s">
         <v>3031</v>
       </c>
       <c r="P11">
@@ -62192,7 +62194,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" ht="51" spans="1:33">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -62235,7 +62237,7 @@
       <c r="N12" t="s">
         <v>38</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="3" t="s">
         <v>3066</v>
       </c>
       <c r="P12">

</xml_diff>